<commit_message>
chore: Add code for graph creation and data processing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mypython\math_modeling\power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC7135-A639-49C3-BE99-492C07C5F96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA43010-E141-417E-8F3E-276FB99E5B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -81,11 +81,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -411,17 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -436,7 +436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -454,7 +454,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -472,7 +472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -490,7 +490,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -498,17 +498,17 @@
         <v>130</v>
       </c>
       <c r="C5">
+        <v>160</v>
+      </c>
+      <c r="D5">
         <v>10</v>
-      </c>
-      <c r="D5">
-        <v>160</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -524,24 +524,6 @@
       <c r="E6">
         <f t="shared" si="0"/>
         <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>SUM(B2:B6)</f>
-        <v>790</v>
-      </c>
-      <c r="C7">
-        <f>SUM(C2:C6)</f>
-        <v>430</v>
-      </c>
-      <c r="D7">
-        <f>SUM(D2:D6)</f>
-        <v>410</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -555,13 +537,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DDCED9-1C79-4FE1-A144-9C73986590F8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -569,10 +551,10 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -594,7 +576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -605,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -616,7 +598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>

</xml_diff>